<commit_message>
I made changes in signin page and tree page.
</commit_message>
<xml_diff>
--- a/src/test/resources/InputData/TestData.xlsx
+++ b/src/test/resources/InputData/TestData.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathvik_balla/Desktop/GithubNew/DSAlgo/src/test/resources/InputData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7526B788-3EB4-B245-A980-18D21A5D85BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="18080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="pythonCode" sheetId="2" r:id="rId5"/>
-    <sheet name="registration" sheetId="3" r:id="rId6"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
+    <sheet name="registration" sheetId="3" r:id="rId3"/>
+    <sheet name="SignIn" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -221,14 +231,23 @@
   <si>
     <t>kkk098</t>
   </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Dsalgo@1</t>
+  </si>
+  <si>
+    <t>sonali</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -246,19 +265,9 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color indexed="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -280,6 +289,18 @@
       <sz val="11"/>
       <color indexed="18"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -428,118 +449,154 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff00cdb2"/>
-      <rgbColor rgb="ff800000"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="015E88B1"/>
+      <rgbColor rgb="01EEF3F4"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF00CDB2"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -741,7 +798,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -760,7 +817,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -790,7 +847,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -816,7 +873,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -842,7 +899,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -868,7 +925,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -894,7 +951,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -920,7 +977,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -946,7 +1003,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -972,7 +1029,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -998,7 +1055,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1011,9 +1068,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1030,7 +1093,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1049,7 +1112,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1075,7 +1138,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1101,7 +1164,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1127,7 +1190,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1153,7 +1216,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1179,7 +1242,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1205,7 +1268,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1231,7 +1294,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1257,7 +1320,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1283,7 +1346,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1296,9 +1359,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1312,7 +1381,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1331,7 +1400,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1361,7 +1430,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1387,7 +1456,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1413,7 +1482,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1439,7 +1508,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1465,7 +1534,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1491,7 +1560,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1517,7 +1586,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1543,7 +1612,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1569,7 +1638,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1582,74 +1651,82 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="13" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="4" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="3" spans="2:4" ht="50" customHeight="1">
+      <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="7" spans="2:4" ht="19">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+    <row r="9" spans="2:4" ht="16">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:4" ht="16">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
+    <row r="11" spans="2:4" ht="16">
+      <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" ht="16">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D12" t="s" s="5">
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1658,157 +1735,158 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'pythonCode'!R1C1" tooltip="" display="pythonCode"/>
-    <hyperlink ref="D12" location="'registration'!R1C1" tooltip="" display="registration"/>
+    <hyperlink ref="D10" location="'pythonCode'!R1C1" display="pythonCode" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D12" location="'registration'!R1C1" display="registration" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="40.7891" style="6" customWidth="1"/>
-    <col min="2" max="2" width="49.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="32.7969" style="6" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="5" customWidth="1"/>
+    <col min="4" max="6" width="8.83203125" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="7">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s" s="7">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="7">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="9">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s" s="9">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" ht="122.55" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="122.5" customHeight="1">
+      <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="122.55" customHeight="1">
-      <c r="A5" t="s" s="13">
+      <c r="C4" s="11"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="122.5" customHeight="1">
+      <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="14">
+      <c r="B5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="137.55" customHeight="1">
-      <c r="A6" t="s" s="13">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="137.5" customHeight="1">
+      <c r="A6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s" s="14">
+      <c r="B6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="15">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s" s="15">
+      <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" t="s" s="7">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="17" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s" s="16">
+      <c r="B8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="91.55" customHeight="1">
-      <c r="A9" t="s" s="17">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="91.5" customHeight="1">
+      <c r="A9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s" s="7">
+      <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="91.55" customHeight="1">
-      <c r="A10" t="s" s="17">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="91.5" customHeight="1">
+      <c r="A10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s" s="7">
+      <c r="B10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s" s="19">
+      <c r="C10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" ht="247.55" customHeight="1">
-      <c r="A11" t="s" s="17">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="247.5" customHeight="1">
+      <c r="A11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s" s="7">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1816,165 +1894,199 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9" style="20" customWidth="1"/>
-    <col min="2" max="5" width="8.85156" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="20" customWidth="1"/>
+    <col min="1" max="1" width="9" style="5" customWidth="1"/>
+    <col min="2" max="6" width="8.83203125" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="21">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s" s="7">
+      <c r="B1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s" s="7">
+      <c r="C1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s" s="7">
+      <c r="D1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="21">
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="22">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="21">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s" s="7">
+      <c r="C4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s" s="7">
+      <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="21">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s" s="7">
+      <c r="C5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s" s="7">
+      <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="21">
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" t="s" s="7">
+      <c r="D6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="21">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A7" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="B7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s" s="7">
+      <c r="C7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="s" s="7">
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="21">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A8" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="B8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="C8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D8" t="s" s="7">
+      <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="270.75" customHeight="1">
-      <c r="A9" t="s" s="21">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="270.75" customHeight="1">
+      <c r="A9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="B9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s" s="7">
+      <c r="C9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D9" t="s" s="7">
+      <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A10" s="20"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE8E04A-D8E9-3142-B404-CD18DCC32B7B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B50AEBBE-8173-3640-8561-5BEF7C2809BB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modifications for all tests
</commit_message>
<xml_diff>
--- a/src/test/resources/InputData/TestData.xlsx
+++ b/src/test/resources/InputData/TestData.xlsx
@@ -1,29 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathvik_balla/Desktop/GithubNew/DSAlgo/src/test/resources/InputData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7526B788-3EB4-B245-A980-18D21A5D85BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="18080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
-    <sheet name="registration" sheetId="3" r:id="rId3"/>
-    <sheet name="SignIn" sheetId="4" r:id="rId4"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
+    <sheet name="pythonCode" sheetId="2" r:id="rId5"/>
+    <sheet name="registration" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -55,13 +45,13 @@
     <t>print"valid code"</t>
   </si>
   <si>
-    <t>pass</t>
+    <t>valid code</t>
   </si>
   <si>
     <t>Print"invalid code"</t>
   </si>
   <si>
-    <t>fail</t>
+    <t>SyntaxError: bad input on line 1</t>
   </si>
   <si>
     <t># This program adds two numbers
@@ -108,9 +98,6 @@
   </si>
   <si>
     <t>print A"rrays in Python"</t>
-  </si>
-  <si>
-    <t>SyntaxError: bad input on line 1</t>
   </si>
   <si>
     <t>def search(input_list, num):
@@ -181,12 +168,21 @@
     <t>Status</t>
   </si>
   <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
     <t>ab%cd$</t>
   </si>
   <si>
     <t>pwd098</t>
   </si>
   <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
     <t>User2</t>
   </si>
   <si>
@@ -220,34 +216,34 @@
     <t>password66</t>
   </si>
   <si>
+    <t xml:space="preserve">MyNameIsIncorrectPassword.DoNotTryMeToCorrect.ToTtestMyTestCaseForMyDS-AlgoProjectAAndHereIamTestingForNegativeScenarioToTestUserNameExceed150Characters. </t>
+  </si>
+  <si>
+    <t>kkk098</t>
+  </si>
+  <si>
     <t>User7</t>
   </si>
   <si>
     <t>Test1177</t>
   </si>
   <si>
-    <t xml:space="preserve">MyNameIsIncorrectPassword.DoNotTryMeToCorrect.ToTtestMyTestCaseForMyDS-AlgoProjectAAndHereIamTestingForNegativeScenarioToTestUserNameExceed150Characters. </t>
-  </si>
-  <si>
-    <t>kkk098</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>sonali</t>
   </si>
   <si>
     <t>Dsalgo@1</t>
-  </si>
-  <si>
-    <t>sonali</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -265,10 +261,25 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color indexed="8"/>
+      <name val="Courier"/>
     </font>
     <font>
       <sz val="13"/>
@@ -281,26 +292,9 @@
       <name val="Menlo Regular"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color indexed="8"/>
-      <name val="Courier"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="18"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -449,154 +443,115 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="015E88B1"/>
-      <rgbColor rgb="01EEF3F4"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FF3F3F3F"/>
-      <rgbColor rgb="FFDBDBDB"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FF00CDB2"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="015e88b1"/>
+      <rgbColor rgb="01eef3f4"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff00cdb2"/>
+      <rgbColor rgb="ff800000"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -798,7 +753,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -817,7 +772,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -847,7 +802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -873,7 +828,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,7 +854,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -925,7 +880,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -951,7 +906,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -977,7 +932,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1003,7 +958,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1029,7 +984,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1010,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1068,15 +1023,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1093,7 +1042,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1112,7 +1061,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1138,7 +1087,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1113,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1190,7 +1139,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1216,7 +1165,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1242,7 +1191,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1268,7 +1217,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1294,7 +1243,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1320,7 +1269,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1346,7 +1295,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1359,15 +1308,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1381,7 +1324,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1400,7 +1343,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1430,7 +1373,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1456,7 +1399,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1482,7 +1425,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1508,7 +1451,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1534,7 +1477,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1560,7 +1503,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1586,7 +1529,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1612,7 +1555,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1638,7 +1581,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1651,83 +1594,75 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D12"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5" customWidth="1"/>
+    <col min="2" max="4" width="30.5547" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="50" customHeight="1">
-      <c r="B3" s="21" t="s">
+    <row r="3" ht="50" customHeight="1">
+      <c r="B3" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-    </row>
-    <row r="7" spans="2:4" ht="19">
-      <c r="B7" s="1" t="s">
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="16">
-      <c r="B9" s="2" t="s">
+    <row r="9">
+      <c r="B9" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="2:4" ht="16">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="16">
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:4" ht="16">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+    <row r="11">
+      <c r="B11" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>31</v>
+      <c r="D12" t="s" s="5">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1735,158 +1670,157 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'pythonCode'!R1C1" display="pythonCode" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D12" location="'registration'!R1C1" display="registration" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D10" location="'pythonCode'!R1C1" tooltip="" display="pythonCode"/>
+    <hyperlink ref="D12" location="'registration'!R1C1" tooltip="" display="registration"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="5" customWidth="1"/>
-    <col min="4" max="6" width="8.83203125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="40.7891" style="6" customWidth="1"/>
+    <col min="2" max="2" width="49.375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="32.7969" style="6" customWidth="1"/>
+    <col min="4" max="5" width="8.85156" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" t="s" s="7">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" ht="22" customHeight="1">
+      <c r="A2" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s" s="9">
         <v>10</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="10">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" ht="122.5" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" ht="122.55" customHeight="1">
+      <c r="A4" t="s" s="11">
         <v>13</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s" s="12">
         <v>14</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="122.5" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" ht="122.55" customHeight="1">
+      <c r="A5" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" ht="137.5" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" ht="137.55" customHeight="1">
+      <c r="A6" t="s" s="14">
         <v>17</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A7" s="14" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" t="s" s="16">
         <v>19</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" ht="17" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="17" customHeight="1">
+      <c r="A8" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" t="s" s="17">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="91.55" customHeight="1">
+      <c r="A9" t="s" s="18">
         <v>22</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" ht="91.5" customHeight="1">
-      <c r="A9" s="16" t="s">
+      <c r="B9" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="91.55" customHeight="1">
+      <c r="A10" t="s" s="18">
         <v>25</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" ht="91.5" customHeight="1">
-      <c r="A10" s="16" t="s">
+      <c r="B10" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" t="s" s="19">
         <v>27</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" ht="247.55" customHeight="1">
+      <c r="A11" t="s" s="18">
         <v>28</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" ht="247.5" customHeight="1">
-      <c r="A11" s="16" t="s">
+      <c r="B11" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1894,199 +1828,190 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9" style="5" customWidth="1"/>
-    <col min="2" max="6" width="8.83203125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="19.3594" style="20" customWidth="1"/>
+    <col min="2" max="2" width="15.2109" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.7891" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="20" customWidth="1"/>
+    <col min="5" max="5" width="60.1641" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" t="s" s="21">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s" s="7">
         <v>32</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" t="s" s="7">
         <v>33</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" t="s" s="7">
         <v>35</v>
       </c>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A2" s="18" t="s">
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="21">
         <v>36</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="D2" t="s" s="7">
         <v>38</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="E2" t="s" s="7">
         <v>39</v>
       </c>
-      <c r="C3" s="6" t="s">
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="22">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s" s="7">
         <v>39</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A5" s="18" t="s">
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" t="s" s="21">
         <v>42</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B4" t="s" s="7">
         <v>43</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C4" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" t="s" s="21">
         <v>44</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A6" s="18" t="s">
+      <c r="B5" t="s" s="7">
         <v>45</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C5" t="s" s="7">
         <v>46</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A7" s="18" t="s">
+      <c r="D5" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" t="s" s="21">
         <v>47</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B6" t="s" s="7">
         <v>48</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C6" t="s" s="7">
         <v>48</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A8" s="18" t="s">
+      <c r="D6" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" t="s" s="21">
         <v>49</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B7" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C7" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" ht="270.75" customHeight="1">
-      <c r="A9" s="18" t="s">
+      <c r="D7" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" ht="104.55" customHeight="1">
+      <c r="A8" t="s" s="21">
         <v>51</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B8" t="s" s="7">
         <v>52</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C8" t="s" s="7">
         <v>52</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="D8" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" t="s" s="21">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s" s="7">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s" s="7">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" t="s" s="21">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE8E04A-D8E9-3142-B404-CD18DCC32B7B}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B50AEBBE-8173-3640-8561-5BEF7C2809BB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new tests for Array, Register, Linked list. Added exception Handling
</commit_message>
<xml_diff>
--- a/src/test/resources/InputData/TestData.xlsx
+++ b/src/test/resources/InputData/TestData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -100,6 +100,33 @@
     <t>print A"rrays in Python"</t>
   </si>
   <si>
+    <t>print "Applications of Array"</t>
+  </si>
+  <si>
+    <t>Applications of Array</t>
+  </si>
+  <si>
+    <t>print A"pplications of Array"</t>
+  </si>
+  <si>
+    <t>print "Basic Operations In Lists"</t>
+  </si>
+  <si>
+    <t>Basic Operations In Lists</t>
+  </si>
+  <si>
+    <t>print B"asic Operations In Lists"</t>
+  </si>
+  <si>
+    <t>print "Arrays Using List”</t>
+  </si>
+  <si>
+    <t>Arrays Using List</t>
+  </si>
+  <si>
+    <t>print A"rrays Using List”</t>
+  </si>
+  <si>
     <t>def search(input_list, num):
 if num in input_list :
 print("Element Found")
@@ -127,30 +154,6 @@
   <si>
     <t xml:space="preserve">Error occurred during submission
 </t>
-  </si>
-  <si>
-    <t>def findMaxConsecutiveOnes(nums) :
-count = 0
-result = 0
-for i in range(0, len(nums)):
-if (nums[i] == 0):
-count = 0
-\b
-\b
-else:
-count+= 1
-\b
-\b
-result = max(result, count)
-\b
-\b
-print(result)
-\b
-\b
-findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>registration</t>
@@ -244,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -287,13 +290,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color indexed="17"/>
-      <name val="Menlo Regular"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="18"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -329,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -442,13 +440,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -500,8 +513,11 @@
     <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
@@ -515,7 +531,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -543,7 +559,6 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff00cdb2"/>
       <rgbColor rgb="ff800000"/>
     </indexedColors>
   </colors>
@@ -1651,7 +1666,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s" s="3">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1662,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1678,7 +1693,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1763,60 +1778,115 @@
       <c r="A7" t="s" s="16">
         <v>19</v>
       </c>
-      <c r="B7" t="s" s="16">
+      <c r="B7" t="s" s="17">
         <v>20</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" t="s" s="7">
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" t="s" s="18">
         <v>21</v>
       </c>
-      <c r="B8" t="s" s="17">
+      <c r="B8" t="s" s="16">
         <v>12</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="91.55" customHeight="1">
-      <c r="A9" t="s" s="18">
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" t="s" s="16">
         <v>22</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="B9" t="s" s="18">
         <v>23</v>
       </c>
-      <c r="C9" t="s" s="7">
-        <v>24</v>
-      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" ht="91.55" customHeight="1">
+    <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="18">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s" s="19">
-        <v>27</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B10" t="s" s="17">
+        <v>12</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" ht="247.55" customHeight="1">
-      <c r="A11" t="s" s="18">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s" s="7">
-        <v>29</v>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" t="s" s="16">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s" s="17">
+        <v>26</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
+    </row>
+    <row r="12" ht="13.55" customHeight="1">
+      <c r="A12" t="s" s="18">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s" s="17">
+        <v>12</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" ht="13.55" customHeight="1">
+      <c r="A13" t="s" s="16">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s" s="17">
+        <v>29</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" ht="13.55" customHeight="1">
+      <c r="A14" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s" s="16">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" ht="91.55" customHeight="1">
+      <c r="A15" t="s" s="19">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" ht="91.55" customHeight="1">
+      <c r="A16" t="s" s="19">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s" s="20">
+        <v>36</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1835,173 +1905,173 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3594" style="20" customWidth="1"/>
-    <col min="2" max="2" width="15.2109" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.7891" style="20" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="20" customWidth="1"/>
-    <col min="5" max="5" width="60.1641" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="20" customWidth="1"/>
+    <col min="1" max="1" width="19.3594" style="21" customWidth="1"/>
+    <col min="2" max="2" width="15.2109" style="21" customWidth="1"/>
+    <col min="3" max="3" width="17.7891" style="21" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="21" customWidth="1"/>
+    <col min="5" max="5" width="60.1641" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="21">
-        <v>31</v>
+      <c r="A1" t="s" s="22">
+        <v>38</v>
       </c>
       <c r="B1" t="s" s="7">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s" s="7">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s" s="7">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s" s="7">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="21">
-        <v>36</v>
+      <c r="A2" t="s" s="22">
+        <v>43</v>
       </c>
       <c r="B2" t="s" s="7">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s" s="7">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s" s="7">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s" s="7">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="22">
-        <v>40</v>
+      <c r="A3" t="s" s="23">
+        <v>47</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s" s="7">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s" s="7">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="21">
-        <v>42</v>
+      <c r="A4" t="s" s="22">
+        <v>49</v>
       </c>
       <c r="B4" t="s" s="7">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s" s="7">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="21">
-        <v>44</v>
+      <c r="A5" t="s" s="22">
+        <v>51</v>
       </c>
       <c r="B5" t="s" s="7">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s" s="7">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s" s="7">
         <v>45</v>
       </c>
-      <c r="C5" t="s" s="7">
+      <c r="E5" t="s" s="7">
         <v>46</v>
       </c>
-      <c r="D5" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s" s="7">
-        <v>39</v>
-      </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="21">
-        <v>47</v>
+      <c r="A6" t="s" s="22">
+        <v>54</v>
       </c>
       <c r="B6" t="s" s="7">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s" s="7">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s" s="7">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="21">
-        <v>49</v>
+      <c r="A7" t="s" s="22">
+        <v>56</v>
       </c>
       <c r="B7" t="s" s="7">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s" s="7">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s" s="7">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" ht="104.55" customHeight="1">
-      <c r="A8" t="s" s="21">
-        <v>51</v>
+      <c r="A8" t="s" s="22">
+        <v>58</v>
       </c>
       <c r="B8" t="s" s="7">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s" s="7">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s" s="7">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="21">
-        <v>53</v>
+      <c r="A9" t="s" s="22">
+        <v>60</v>
       </c>
       <c r="B9" t="s" s="7">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s" s="7">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s" s="7">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="21">
-        <v>56</v>
+      <c r="A10" t="s" s="22">
+        <v>63</v>
       </c>
       <c r="B10" t="s" s="7">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>

</xml_diff>